<commit_message>
added success and error popups
</commit_message>
<xml_diff>
--- a/backend/vsrs.xlsx
+++ b/backend/vsrs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="90">
   <si>
     <t>_id</t>
   </si>
@@ -28,6 +28,9 @@
     <t>maritalStatus</t>
   </si>
   <si>
+    <t>spouseName</t>
+  </si>
+  <si>
     <t>agesOfBoys</t>
   </si>
   <si>
@@ -79,9 +82,6 @@
     <t>lastRank</t>
   </si>
   <si>
-    <t>militaryId</t>
-  </si>
-  <si>
     <t>petCompanion</t>
   </si>
   <si>
@@ -112,172 +112,175 @@
     <t>lastUpdated</t>
   </si>
   <si>
-    <t>status</t>
+    <t>__v</t>
   </si>
   <si>
     <t>selectedFurnitureItems</t>
   </si>
   <si>
-    <t>"65dc11c9e5dcfed83ecf1f65"</t>
-  </si>
-  <si>
-    <t>Benjamin Johnson</t>
+    <t>"65ea22f9931d4595e68d8e48"</t>
+  </si>
+  <si>
+    <t>Justin Timberlake</t>
   </si>
   <si>
     <t>Male</t>
   </si>
   <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>Jane Timberlake</t>
+  </si>
+  <si>
+    <t>[5,10]</t>
+  </si>
+  <si>
+    <t>[6]</t>
+  </si>
+  <si>
+    <t>["Asian"]</t>
+  </si>
+  <si>
+    <t>Employed</t>
+  </si>
+  <si>
+    <t>$12,500 and under</t>
+  </si>
+  <si>
+    <t>House</t>
+  </si>
+  <si>
+    <t>9500 Gilman Drive</t>
+  </si>
+  <si>
+    <t>San Diego</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>testing@gmail.com</t>
+  </si>
+  <si>
+    <t>["Air Force"]</t>
+  </si>
+  <si>
+    <t>["WWII","Special Ops"]</t>
+  </si>
+  <si>
+    <t>General Under Honorable</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Colleague</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>"65efb333260e72406b1f2f74"</t>
+  </si>
+  <si>
     <t>Single</t>
   </si>
   <si>
-    <t>[2,9,5]</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>["Caucasian","Other","Asian"]</t>
-  </si>
-  <si>
-    <t>In School</t>
-  </si>
-  <si>
-    <t>$12,500 and under</t>
+    <t/>
+  </si>
+  <si>
+    <t>1111 TSE Lane</t>
+  </si>
+  <si>
+    <t>123-456-7890</t>
+  </si>
+  <si>
+    <t>tsepapdev@gmail.com</t>
+  </si>
+  <si>
+    <t>Still Serving</t>
+  </si>
+  <si>
+    <t>Officer</t>
+  </si>
+  <si>
+    <t>Social Media</t>
+  </si>
+  <si>
+    <t>[{"furnitureItemId":"65efb2737bd85fd77c477c33","quantity":1,"_id":"65efb333260e72406b1f2f75"},{"furnitureItemId":"65efb2737bd85fd77c477c3a","quantity":1,"_id":"65efb333260e72406b1f2f76"},{"furnitureItemId":"65efb2737bd85fd77c477c3e","quantity":0,"_id":"65efb333260e72406b1f2f77"},{"furnitureItemId":"65efb2737bd85fd77c477c42","quantity":1,"_id":"65efb333260e72406b1f2f78"},{"furnitureItemId":"65efb2737bd85fd77c477c43","quantity":0,"_id":"65efb333260e72406b1f2f79"},{"furnitureItemId":"65efb2737bd85fd77c477c48","quantity":1,"_id":"65efb333260e72406b1f2f7a"},{"furnitureItemId":"65efb2737bd85fd77c477c4c","quantity":1,"_id":"65efb333260e72406b1f2f7b"},{"furnitureItemId":"65efb2737bd85fd77c477c55","quantity":1,"_id":"65efb333260e72406b1f2f7c"},{"furnitureItemId":"65efb2737bd85fd77c477c4d","quantity":3,"_id":"65efb333260e72406b1f2f7d"},{"furnitureItemId":"65efb2737bd85fd77c477c4e","quantity":0,"_id":"65efb333260e72406b1f2f7e"},{"furnitureItemId":"65efb2737bd85fd77c477c57","quantity":3,"_id":"65efb333260e72406b1f2f7f"},{"furnitureItemId":"65efb2737bd85fd77c477c58","quantity":1,"_id":"65efb333260e72406b1f2f80"}]</t>
+  </si>
+  <si>
+    <t>"65efb566260e72406b1f2fee"</t>
+  </si>
+  <si>
+    <t>Pap Dev</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Widowed/Widower</t>
+  </si>
+  <si>
+    <t>[16]</t>
+  </si>
+  <si>
+    <t>[13,8]</t>
+  </si>
+  <si>
+    <t>["Middle Eastern"]</t>
+  </si>
+  <si>
+    <t>Currently Looking</t>
+  </si>
+  <si>
+    <t>$25,001 - $50,000</t>
+  </si>
+  <si>
+    <t>3 Bedroom</t>
+  </si>
+  <si>
+    <t>[{"furnitureItemId":"65efb2737bd85fd77c477c3e","quantity":0,"_id":"65efb566260e72406b1f2fef"},{"furnitureItemId":"65efb2737bd85fd77c477c3b","quantity":0,"_id":"65efb566260e72406b1f2ff0"},{"furnitureItemId":"65efb2737bd85fd77c477c3c","quantity":0,"_id":"65efb566260e72406b1f2ff1"},{"furnitureItemId":"65efb2737bd85fd77c477c4c","quantity":0,"_id":"65efb566260e72406b1f2ff2"},{"furnitureItemId":"65efb2737bd85fd77c477c4b","quantity":0,"_id":"65efb566260e72406b1f2ff3"},{"furnitureItemId":"65efb2737bd85fd77c477c50","quantity":0,"_id":"65efb566260e72406b1f2ff4"},{"furnitureItemId":"65efb2737bd85fd77c477c58","quantity":1,"_id":"65efb566260e72406b1f2ff5"},{"furnitureItemId":"65efb2737bd85fd77c477c5b","quantity":0,"_id":"65efb566260e72406b1f2ff6"},{"furnitureItemId":"65efb2737bd85fd77c477c5a","quantity":0,"_id":"65efb566260e72406b1f2ff7"}]</t>
+  </si>
+  <si>
+    <t>"65f08a337841eeba03786dbf"</t>
+  </si>
+  <si>
+    <t>Samvrit Srinath</t>
   </si>
   <si>
     <t>Apartment</t>
   </si>
   <si>
-    <t>1234 TSE Lane</t>
-  </si>
-  <si>
-    <t>La Jolla</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>111-111-1111</t>
-  </si>
-  <si>
-    <t>tsepapdev@gmail.com</t>
-  </si>
-  <si>
-    <t>["Navy","Air Force"]</t>
-  </si>
-  <si>
-    <t>["Test Conflict"]</t>
-  </si>
-  <si>
-    <t>Still Serving</t>
-  </si>
-  <si>
-    <t>Officer</t>
-  </si>
-  <si>
-    <t>Internet</t>
-  </si>
-  <si>
-    <t>Approved</t>
-  </si>
-  <si>
-    <t>"65f3d78730e000f584340d04"</t>
-  </si>
-  <si>
-    <t>Steven D. Shi</t>
-  </si>
-  <si>
-    <t>[2,4,3,1]</t>
-  </si>
-  <si>
-    <t>["Asian"]</t>
-  </si>
-  <si>
-    <t>Employed</t>
-  </si>
-  <si>
-    <t>$12,501 - $25,000</t>
-  </si>
-  <si>
-    <t>8252 BENT TREE LN</t>
-  </si>
-  <si>
-    <t>Jurupa Valley</t>
-  </si>
-  <si>
-    <t>GA</t>
-  </si>
-  <si>
-    <t>3109864429</t>
-  </si>
-  <si>
-    <t>stevendiwenshi1113@gmail.com</t>
-  </si>
-  <si>
-    <t>["Coast Guard"]</t>
-  </si>
-  <si>
-    <t>["Korea"]</t>
+    <t>[{"furnitureItemId":"65efb2737bd85fd77c477c4b","quantity":1,"_id":"65f08a337841eeba03786dc0"},{"furnitureItemId":"65efb2737bd85fd77c477c51","quantity":1,"_id":"65f08a337841eeba03786dc1"}]</t>
+  </si>
+  <si>
+    <t>"65f0de3cebad9e8c9e20cda7"</t>
+  </si>
+  <si>
+    <t>Harsh Gurnani</t>
+  </si>
+  <si>
+    <t>asidkjfas</t>
+  </si>
+  <si>
+    <t>kdajfsdl</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>9258209192</t>
+  </si>
+  <si>
+    <t>["WWII"]</t>
   </si>
   <si>
     <t>Honorable Discharge</t>
-  </si>
-  <si>
-    <t>Admiral</t>
-  </si>
-  <si>
-    <t>Colleague</t>
-  </si>
-  <si>
-    <t>Received</t>
-  </si>
-  <si>
-    <t>"65f3d80230e000f584340d08"</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Married</t>
-  </si>
-  <si>
-    <t>["Native American"]</t>
-  </si>
-  <si>
-    <t>Retired</t>
-  </si>
-  <si>
-    <t>$25,001 - $50,000</t>
-  </si>
-  <si>
-    <t>4+ Bedroom</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>asdfjksdhfjskhfkjsdfksjf</t>
-  </si>
-  <si>
-    <t>stevendiwenshi1</t>
-  </si>
-  <si>
-    <t>["Army"]</t>
-  </si>
-  <si>
-    <t>["Panama"]</t>
-  </si>
-  <si>
-    <t>Bad Conduct</t>
-  </si>
-  <si>
-    <t>Admirajjo</t>
-  </si>
-  <si>
-    <t>hhhhh</t>
   </si>
 </sst>
 </file>
@@ -655,7 +658,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI4"/>
+  <dimension ref="A1:AI6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="35" width="20" customWidth="1"/>
@@ -811,11 +814,11 @@
       <c r="N2" t="s">
         <v>47</v>
       </c>
-      <c r="O2">
-        <v>92000</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="O2" t="s">
         <v>48</v>
+      </c>
+      <c r="P2">
+        <v>92093</v>
       </c>
       <c r="Q2" t="s">
         <v>49</v>
@@ -829,58 +832,58 @@
       <c r="T2" t="s">
         <v>52</v>
       </c>
-      <c r="U2" t="b">
+      <c r="U2" t="s">
+        <v>53</v>
+      </c>
+      <c r="V2" t="b">
         <v>1</v>
       </c>
-      <c r="V2" t="s">
-        <v>53</v>
-      </c>
-      <c r="W2">
-        <v>1111</v>
+      <c r="W2" t="s">
+        <v>54</v>
       </c>
       <c r="X2" t="b">
         <v>1</v>
       </c>
       <c r="Y2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Z2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="AA2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="AB2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="AC2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="AD2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="AE2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="AF2" s="1">
-        <v>45348.18159270834</v>
+        <v>45358.851778958335</v>
       </c>
       <c r="AG2" s="1">
-        <v>45348.18159270834</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>55</v>
+        <v>45358.851778958335</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
       </c>
       <c r="AI2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>37</v>
@@ -889,162 +892,355 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I3" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="J3" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="K3" t="s">
         <v>44</v>
       </c>
       <c r="L3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3">
+        <v>92122</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>61</v>
+      </c>
+      <c r="R3" t="s">
         <v>62</v>
       </c>
-      <c r="M3" t="s">
+      <c r="S3" t="s">
+        <v>56</v>
+      </c>
+      <c r="T3" t="s">
+        <v>56</v>
+      </c>
+      <c r="U3" t="s">
         <v>63</v>
       </c>
-      <c r="N3" t="s">
+      <c r="V3" t="b">
+        <v>1</v>
+      </c>
+      <c r="W3" t="s">
         <v>64</v>
-      </c>
-      <c r="O3">
-        <v>90277</v>
-      </c>
-      <c r="P3" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>66</v>
-      </c>
-      <c r="R3" t="s">
-        <v>67</v>
-      </c>
-      <c r="S3" t="s">
-        <v>68</v>
-      </c>
-      <c r="T3" t="s">
-        <v>69</v>
-      </c>
-      <c r="U3" t="b">
-        <v>1</v>
-      </c>
-      <c r="V3" t="s">
-        <v>70</v>
       </c>
       <c r="X3" t="b">
         <v>1</v>
       </c>
       <c r="Y3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="AF3" s="1">
-        <v>45366.21341434028</v>
+        <v>45363.07170211806</v>
       </c>
       <c r="AG3" s="1">
-        <v>45366.21341434028</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>72</v>
+        <v>45363.07170211806</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
       </c>
       <c r="AI3" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" t="s">
         <v>73</v>
       </c>
-      <c r="B4" t="s">
+      <c r="J4" t="s">
         <v>74</v>
       </c>
-      <c r="C4" t="s">
+      <c r="K4" t="s">
         <v>75</v>
       </c>
-      <c r="D4">
-        <v>160</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="L4" t="s">
         <v>76</v>
       </c>
-      <c r="F4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="M4" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" t="s">
+        <v>48</v>
+      </c>
+      <c r="P4">
+        <v>92122</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>61</v>
+      </c>
+      <c r="R4" t="s">
+        <v>62</v>
+      </c>
+      <c r="S4" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4" t="s">
+        <v>56</v>
+      </c>
+      <c r="U4" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" t="b">
+        <v>1</v>
+      </c>
+      <c r="W4" t="s">
+        <v>64</v>
+      </c>
+      <c r="X4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>45363.07822429398</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>45363.07822429398</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4" t="s">
         <v>77</v>
       </c>
-      <c r="I4" t="s">
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>78</v>
       </c>
-      <c r="J4" t="s">
+      <c r="B5" t="s">
         <v>79</v>
       </c>
-      <c r="K4" t="s">
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" t="s">
         <v>80</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N5" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5" t="s">
+        <v>48</v>
+      </c>
+      <c r="P5">
+        <v>92122</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R5" t="s">
         <v>62</v>
       </c>
-      <c r="M4" t="s">
+      <c r="S5" t="s">
+        <v>56</v>
+      </c>
+      <c r="T5" t="s">
+        <v>56</v>
+      </c>
+      <c r="U5" t="s">
         <v>63</v>
       </c>
-      <c r="N4" t="s">
+      <c r="V5" t="b">
+        <v>1</v>
+      </c>
+      <c r="W5" t="s">
+        <v>64</v>
+      </c>
+      <c r="X5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>45363.708740358794</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>45363.708740358794</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5" t="s">
         <v>81</v>
       </c>
-      <c r="O4">
-        <v>90222</v>
-      </c>
-      <c r="P4" t="s">
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>82</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="B6" t="s">
         <v>83</v>
       </c>
-      <c r="R4" t="s">
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" t="s">
         <v>84</v>
       </c>
-      <c r="S4" t="s">
+      <c r="N6" t="s">
         <v>85</v>
       </c>
-      <c r="T4" t="s">
+      <c r="O6" t="s">
         <v>86</v>
       </c>
-      <c r="U4" t="b">
+      <c r="P6">
+        <v>94353</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>87</v>
+      </c>
+      <c r="R6" t="s">
+        <v>62</v>
+      </c>
+      <c r="S6" t="s">
+        <v>51</v>
+      </c>
+      <c r="T6" t="s">
+        <v>88</v>
+      </c>
+      <c r="U6" t="s">
+        <v>89</v>
+      </c>
+      <c r="V6" t="b">
         <v>1</v>
       </c>
-      <c r="V4" t="s">
-        <v>87</v>
-      </c>
-      <c r="X4" t="b">
+      <c r="W6" t="s">
+        <v>54</v>
+      </c>
+      <c r="X6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>45363.95773875</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>45363.95773875</v>
+      </c>
+      <c r="AH6">
         <v>0</v>
       </c>
-      <c r="Y4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF4" s="1">
-        <v>45366.21484672454</v>
-      </c>
-      <c r="AG4" s="1">
-        <v>45366.21484672454</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>40</v>
+      <c r="AI6" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added loading state to export button
</commit_message>
<xml_diff>
--- a/backend/vsrs.xlsx
+++ b/backend/vsrs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="110">
   <si>
     <t>_id</t>
   </si>
@@ -118,7 +118,7 @@
     <t>selectedFurnitureItems</t>
   </si>
   <si>
-    <t>"65ea22f9931d4595e68d8e48"</t>
+    <t>65ea22f9931d4595e68d8e48</t>
   </si>
   <si>
     <t>Justin Timberlake</t>
@@ -133,13 +133,13 @@
     <t>Jane Timberlake</t>
   </si>
   <si>
-    <t>[5,10]</t>
-  </si>
-  <si>
-    <t>[6]</t>
-  </si>
-  <si>
-    <t>["Asian"]</t>
+    <t>5,10</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Asian</t>
   </si>
   <si>
     <t>Employed</t>
@@ -166,33 +166,36 @@
     <t>testing@gmail.com</t>
   </si>
   <si>
-    <t>["Air Force"]</t>
-  </si>
-  <si>
-    <t>["WWII","Special Ops"]</t>
+    <t>Air Force</t>
+  </si>
+  <si>
+    <t>WWII,Special Ops</t>
   </si>
   <si>
     <t>General Under Honorable</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>General</t>
   </si>
   <si>
     <t>Colleague</t>
   </si>
   <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>"65efb333260e72406b1f2f74"</t>
+    <t/>
+  </si>
+  <si>
+    <t>Thu Mar 07 2024 12:26:33 GMT-0800 (Pacific Standard Time)</t>
+  </si>
+  <si>
+    <t>65efb333260e72406b1f2f74</t>
   </si>
   <si>
     <t>Single</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>1111 TSE Lane</t>
   </si>
   <si>
@@ -211,10 +214,13 @@
     <t>Social Media</t>
   </si>
   <si>
-    <t>[{"furnitureItemId":"65efb2737bd85fd77c477c33","quantity":1,"_id":"65efb333260e72406b1f2f75"},{"furnitureItemId":"65efb2737bd85fd77c477c3a","quantity":1,"_id":"65efb333260e72406b1f2f76"},{"furnitureItemId":"65efb2737bd85fd77c477c3e","quantity":0,"_id":"65efb333260e72406b1f2f77"},{"furnitureItemId":"65efb2737bd85fd77c477c42","quantity":1,"_id":"65efb333260e72406b1f2f78"},{"furnitureItemId":"65efb2737bd85fd77c477c43","quantity":0,"_id":"65efb333260e72406b1f2f79"},{"furnitureItemId":"65efb2737bd85fd77c477c48","quantity":1,"_id":"65efb333260e72406b1f2f7a"},{"furnitureItemId":"65efb2737bd85fd77c477c4c","quantity":1,"_id":"65efb333260e72406b1f2f7b"},{"furnitureItemId":"65efb2737bd85fd77c477c55","quantity":1,"_id":"65efb333260e72406b1f2f7c"},{"furnitureItemId":"65efb2737bd85fd77c477c4d","quantity":3,"_id":"65efb333260e72406b1f2f7d"},{"furnitureItemId":"65efb2737bd85fd77c477c4e","quantity":0,"_id":"65efb333260e72406b1f2f7e"},{"furnitureItemId":"65efb2737bd85fd77c477c57","quantity":3,"_id":"65efb333260e72406b1f2f7f"},{"furnitureItemId":"65efb2737bd85fd77c477c58","quantity":1,"_id":"65efb333260e72406b1f2f80"}]</t>
-  </si>
-  <si>
-    <t>"65efb566260e72406b1f2fee"</t>
+    <t>Mon Mar 11 2024 18:43:15 GMT-0700 (Pacific Daylight Time)</t>
+  </si>
+  <si>
+    <t>object Object],[object Object],[object Object],[object Object],[object Object],[object Object],[object Object],[object Object],[object Object],[object Object],[object Object],[object Object</t>
+  </si>
+  <si>
+    <t>65efb566260e72406b1f2fee</t>
   </si>
   <si>
     <t>Pap Dev</t>
@@ -226,13 +232,13 @@
     <t>Widowed/Widower</t>
   </si>
   <si>
-    <t>[16]</t>
-  </si>
-  <si>
-    <t>[13,8]</t>
-  </si>
-  <si>
-    <t>["Middle Eastern"]</t>
+    <t>16</t>
+  </si>
+  <si>
+    <t>13,8</t>
+  </si>
+  <si>
+    <t>Middle Eastern</t>
   </si>
   <si>
     <t>Currently Looking</t>
@@ -244,10 +250,13 @@
     <t>3 Bedroom</t>
   </si>
   <si>
-    <t>[{"furnitureItemId":"65efb2737bd85fd77c477c3e","quantity":0,"_id":"65efb566260e72406b1f2fef"},{"furnitureItemId":"65efb2737bd85fd77c477c3b","quantity":0,"_id":"65efb566260e72406b1f2ff0"},{"furnitureItemId":"65efb2737bd85fd77c477c3c","quantity":0,"_id":"65efb566260e72406b1f2ff1"},{"furnitureItemId":"65efb2737bd85fd77c477c4c","quantity":0,"_id":"65efb566260e72406b1f2ff2"},{"furnitureItemId":"65efb2737bd85fd77c477c4b","quantity":0,"_id":"65efb566260e72406b1f2ff3"},{"furnitureItemId":"65efb2737bd85fd77c477c50","quantity":0,"_id":"65efb566260e72406b1f2ff4"},{"furnitureItemId":"65efb2737bd85fd77c477c58","quantity":1,"_id":"65efb566260e72406b1f2ff5"},{"furnitureItemId":"65efb2737bd85fd77c477c5b","quantity":0,"_id":"65efb566260e72406b1f2ff6"},{"furnitureItemId":"65efb2737bd85fd77c477c5a","quantity":0,"_id":"65efb566260e72406b1f2ff7"}]</t>
-  </si>
-  <si>
-    <t>"65f08a337841eeba03786dbf"</t>
+    <t>Mon Mar 11 2024 18:52:38 GMT-0700 (Pacific Daylight Time)</t>
+  </si>
+  <si>
+    <t>object Object],[object Object],[object Object],[object Object],[object Object],[object Object],[object Object],[object Object],[object Object</t>
+  </si>
+  <si>
+    <t>65f08a337841eeba03786dbf</t>
   </si>
   <si>
     <t>Samvrit Srinath</t>
@@ -256,10 +265,13 @@
     <t>Apartment</t>
   </si>
   <si>
-    <t>[{"furnitureItemId":"65efb2737bd85fd77c477c4b","quantity":1,"_id":"65f08a337841eeba03786dc0"},{"furnitureItemId":"65efb2737bd85fd77c477c51","quantity":1,"_id":"65f08a337841eeba03786dc1"}]</t>
-  </si>
-  <si>
-    <t>"65f0de3cebad9e8c9e20cda7"</t>
+    <t>Tue Mar 12 2024 10:00:35 GMT-0700 (Pacific Daylight Time)</t>
+  </si>
+  <si>
+    <t>object Object],[object Object</t>
+  </si>
+  <si>
+    <t>65f0de3cebad9e8c9e20cda7</t>
   </si>
   <si>
     <t>Harsh Gurnani</t>
@@ -277,10 +289,58 @@
     <t>9258209192</t>
   </si>
   <si>
-    <t>["WWII"]</t>
+    <t>WWII</t>
   </si>
   <si>
     <t>Honorable Discharge</t>
+  </si>
+  <si>
+    <t>Tue Mar 12 2024 15:59:08 GMT-0700 (Pacific Daylight Time)</t>
+  </si>
+  <si>
+    <t>661d5415e6250533bd4bac61</t>
+  </si>
+  <si>
+    <t>Hrithik Pai</t>
+  </si>
+  <si>
+    <t>14,12,10</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Asian,Middle Eastern</t>
+  </si>
+  <si>
+    <t>Unemployed</t>
+  </si>
+  <si>
+    <t>La Jolla</t>
+  </si>
+  <si>
+    <t>5108908845</t>
+  </si>
+  <si>
+    <t>hpai@ucsd.edu</t>
+  </si>
+  <si>
+    <t>Air Force,Air Force Reserve</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>Mon Apr 15 2024 09:21:41 GMT-0700 (Pacific Daylight Time)</t>
+  </si>
+  <si>
+    <t>object Object],[object Object],[object Object],[object Object],[object Object],[object Object],[object Object</t>
   </si>
 </sst>
 </file>
@@ -316,9 +376,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,7 +717,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI6"/>
+  <dimension ref="A1:AI7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="35" width="20" customWidth="1"/>
@@ -835,52 +894,52 @@
       <c r="U2" t="s">
         <v>53</v>
       </c>
-      <c r="V2" t="b">
-        <v>1</v>
+      <c r="V2" t="s">
+        <v>54</v>
       </c>
       <c r="W2" t="s">
+        <v>55</v>
+      </c>
+      <c r="X2" t="s">
         <v>54</v>
       </c>
-      <c r="X2" t="b">
-        <v>1</v>
-      </c>
       <c r="Y2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Z2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AA2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AB2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AC2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AD2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AE2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>45358.851778958335</v>
-      </c>
-      <c r="AG2" s="1">
-        <v>45358.851778958335</v>
+        <v>57</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>58</v>
       </c>
       <c r="AH2">
         <v>0</v>
       </c>
       <c r="AI2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
@@ -892,16 +951,16 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
         <v>42</v>
@@ -916,7 +975,7 @@
         <v>45</v>
       </c>
       <c r="M3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N3" t="s">
         <v>47</v>
@@ -928,81 +987,81 @@
         <v>92122</v>
       </c>
       <c r="Q3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="S3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="T3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="U3" t="s">
-        <v>63</v>
-      </c>
-      <c r="V3" t="b">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="V3" t="s">
+        <v>54</v>
       </c>
       <c r="W3" t="s">
-        <v>64</v>
-      </c>
-      <c r="X3" t="b">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="X3" t="s">
+        <v>54</v>
       </c>
       <c r="Y3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF3" s="1">
-        <v>45363.07170211806</v>
-      </c>
-      <c r="AG3" s="1">
-        <v>45363.07170211806</v>
+        <v>66</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>67</v>
       </c>
       <c r="AH3">
         <v>0</v>
       </c>
       <c r="AI3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D4">
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N4" t="s">
         <v>47</v>
@@ -1014,51 +1073,51 @@
         <v>92122</v>
       </c>
       <c r="Q4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="S4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="T4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="U4" t="s">
-        <v>63</v>
-      </c>
-      <c r="V4" t="b">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="V4" t="s">
+        <v>54</v>
       </c>
       <c r="W4" t="s">
-        <v>64</v>
-      </c>
-      <c r="X4" t="b">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="X4" t="s">
+        <v>54</v>
       </c>
       <c r="Y4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF4" s="1">
-        <v>45363.07822429398</v>
-      </c>
-      <c r="AG4" s="1">
-        <v>45363.07822429398</v>
+        <v>66</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>79</v>
       </c>
       <c r="AH4">
         <v>0</v>
       </c>
       <c r="AI4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -1067,13 +1126,13 @@
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I5" t="s">
         <v>42</v>
@@ -1085,10 +1144,10 @@
         <v>44</v>
       </c>
       <c r="L5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="M5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N5" t="s">
         <v>47</v>
@@ -1100,51 +1159,51 @@
         <v>92122</v>
       </c>
       <c r="Q5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="S5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="T5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="U5" t="s">
-        <v>63</v>
-      </c>
-      <c r="V5" t="b">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="V5" t="s">
+        <v>54</v>
       </c>
       <c r="W5" t="s">
-        <v>64</v>
-      </c>
-      <c r="X5" t="b">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="X5" t="s">
+        <v>54</v>
       </c>
       <c r="Y5" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF5" s="1">
-        <v>45363.708740358794</v>
-      </c>
-      <c r="AG5" s="1">
-        <v>45363.708740358794</v>
+        <v>66</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>84</v>
       </c>
       <c r="AH5">
         <v>0</v>
       </c>
       <c r="AI5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
@@ -1153,13 +1212,13 @@
         <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I6" t="s">
         <v>42</v>
@@ -1174,73 +1233,162 @@
         <v>45</v>
       </c>
       <c r="M6" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="N6" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="O6" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="P6">
         <v>94353</v>
       </c>
       <c r="Q6" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="R6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="S6" t="s">
         <v>51</v>
       </c>
       <c r="T6" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="U6" t="s">
-        <v>89</v>
-      </c>
-      <c r="V6" t="b">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="V6" t="s">
+        <v>54</v>
       </c>
       <c r="W6" t="s">
+        <v>55</v>
+      </c>
+      <c r="X6" t="s">
         <v>54</v>
       </c>
-      <c r="X6" t="b">
-        <v>1</v>
-      </c>
       <c r="Y6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Z6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AA6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AB6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AC6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AD6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AE6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF6" s="1">
-        <v>45363.95773875</v>
-      </c>
-      <c r="AG6" s="1">
-        <v>45363.95773875</v>
+        <v>57</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>94</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>94</v>
       </c>
       <c r="AH6">
         <v>0</v>
       </c>
       <c r="AI6" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I7" t="s">
+        <v>99</v>
+      </c>
+      <c r="J7" t="s">
+        <v>100</v>
+      </c>
+      <c r="K7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" t="s">
+        <v>83</v>
+      </c>
+      <c r="M7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" t="s">
+        <v>101</v>
+      </c>
+      <c r="O7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P7">
+        <v>92093</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>102</v>
+      </c>
+      <c r="R7" t="s">
+        <v>103</v>
+      </c>
+      <c r="S7" t="s">
+        <v>104</v>
+      </c>
+      <c r="T7" t="s">
+        <v>105</v>
+      </c>
+      <c r="U7" t="s">
+        <v>93</v>
+      </c>
+      <c r="V7" t="b">
+        <v>0</v>
+      </c>
+      <c r="W7" t="s">
+        <v>106</v>
+      </c>
+      <c r="X7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>108</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>